<commit_message>
Refactored Code. Extract rules from board. Extracted rules from board into a Rules object
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="32">
   <si>
     <t>W</t>
   </si>
@@ -118,7 +118,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,6 +152,22 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -287,7 +303,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -304,6 +320,8 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -607,10 +625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:O29"/>
+  <dimension ref="B2:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -742,7 +760,7 @@
       <c r="D11" t="s">
         <v>0</v>
       </c>
-      <c r="J11" s="3" t="s">
+      <c r="J11" s="17" t="s">
         <v>9</v>
       </c>
       <c r="M11" t="s">
@@ -854,7 +872,7 @@
       </c>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="J21" s="3" t="s">
+      <c r="J21" s="16" t="s">
         <v>18</v>
       </c>
     </row>
@@ -942,6 +960,39 @@
       </c>
       <c r="C29">
         <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="G31" t="s">
+        <v>1</v>
+      </c>
+      <c r="H31" t="s">
+        <v>1</v>
+      </c>
+      <c r="I31" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="G32" t="s">
+        <v>1</v>
+      </c>
+      <c r="H32" t="s">
+        <v>1</v>
+      </c>
+      <c r="I32" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G33" t="s">
+        <v>1</v>
+      </c>
+      <c r="H33" t="s">
+        <v>1</v>
+      </c>
+      <c r="I33" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>